<commit_message>
[🛠️Fix] Skill balance fix
- 동료, 스킬 소환 확률 수정
- 동료, 스킬 보유효과 수정
- 스킬 전체 밸런스 수정
</commit_message>
<xml_diff>
--- a/IdleGame/Assets/@Resources/Texts/ExcelTable/SummonTable.xlsx
+++ b/IdleGame/Assets/@Resources/Texts/ExcelTable/SummonTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\TeamProject-IdleGame\IdleGame\Assets\@Resources\Texts\ExcelTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC10D0D-4149-4CBF-BF80-DA82F6C80838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D0792F-D634-4BD9-A0C7-CDE69EAC7EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Equipment" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="81">
   <si>
     <t>Probability : Int</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -263,6 +263,24 @@
   </si>
   <si>
     <t>A0025</t>
+  </si>
+  <si>
+    <t>S0010</t>
+  </si>
+  <si>
+    <t>S0011</t>
+  </si>
+  <si>
+    <t>S0012</t>
+  </si>
+  <si>
+    <t>S0013</t>
+  </si>
+  <si>
+    <t>S0014</t>
+  </si>
+  <si>
+    <t>S0015</t>
   </si>
 </sst>
 </file>
@@ -350,8 +368,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EB499717-A1AC-43E5-BB07-2DDEA916DCA8}" name="표1_3" displayName="표1_3" ref="A2:C47" totalsRowShown="0">
-  <autoFilter ref="A2:C47" xr:uid="{EB499717-A1AC-43E5-BB07-2DDEA916DCA8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EB499717-A1AC-43E5-BB07-2DDEA916DCA8}" name="표1_3" displayName="표1_3" ref="A2:C122" totalsRowShown="0">
+  <autoFilter ref="A2:C122" xr:uid="{EB499717-A1AC-43E5-BB07-2DDEA916DCA8}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{06FEEBCF-143F-467A-94A3-ED6516C27AF9}" name="SummonGrade : Int"/>
     <tableColumn id="2" xr3:uid="{94EF72E9-ADB9-4815-8659-1DBA16E8F4CA}" name="ItemId : String" dataDxfId="1"/>
@@ -362,8 +380,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5A4DFF02-36B8-41E7-8806-3F9C3960FF2C}" name="표1_34" displayName="표1_34" ref="A2:C32" totalsRowShown="0">
-  <autoFilter ref="A2:C32" xr:uid="{5A4DFF02-36B8-41E7-8806-3F9C3960FF2C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5A4DFF02-36B8-41E7-8806-3F9C3960FF2C}" name="표1_34" displayName="표1_34" ref="A2:C62" totalsRowShown="0">
+  <autoFilter ref="A2:C62" xr:uid="{5A4DFF02-36B8-41E7-8806-3F9C3960FF2C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{33B2D4D5-FB6D-4D4D-BFB4-929061FDF8C7}" name="SummonGrade : Int"/>
     <tableColumn id="2" xr3:uid="{ED56F630-FCAF-4415-A242-47AC6BE1C32C}" name="ItemId : String" dataDxfId="0"/>
@@ -638,7 +656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D362"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A333" workbookViewId="0">
+    <sheetView topLeftCell="A333" workbookViewId="0">
       <selection activeCell="M348" sqref="M348"/>
     </sheetView>
   </sheetViews>
@@ -2581,7 +2599,7 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163">
-        <f>A147</f>
+        <f t="shared" ref="A163:A173" si="9">A147</f>
         <v>6</v>
       </c>
       <c r="B163" s="1" t="s">
@@ -2593,7 +2611,7 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164">
-        <f>A148</f>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="B164" s="1" t="s">
@@ -2605,7 +2623,7 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165">
-        <f>A149</f>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="B165" s="1" t="s">
@@ -2617,7 +2635,7 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166">
-        <f>A150</f>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="B166" s="1" t="s">
@@ -2629,7 +2647,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167">
-        <f>A151</f>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="B167" s="1" t="s">
@@ -2641,7 +2659,7 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168">
-        <f>A152</f>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="B168" s="1" t="s">
@@ -2653,7 +2671,7 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169">
-        <f>A153</f>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="B169" s="1" t="s">
@@ -2665,7 +2683,7 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170">
-        <f>A154</f>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="B170" s="1" t="s">
@@ -2677,7 +2695,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171">
-        <f>A155</f>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="B171" s="1" t="s">
@@ -2689,7 +2707,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172">
-        <f>A156</f>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="B172" s="1" t="s">
@@ -2701,7 +2719,7 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173">
-        <f>A157</f>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="B173" s="1" t="s">
@@ -2713,7 +2731,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174">
-        <f t="shared" ref="A174:A182" si="9">A163</f>
+        <f t="shared" ref="A174:A182" si="10">A163</f>
         <v>6</v>
       </c>
       <c r="B174" s="1" t="s">
@@ -2725,7 +2743,7 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="B175" s="1" t="s">
@@ -2737,7 +2755,7 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="B176" s="1" t="s">
@@ -2749,7 +2767,7 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="B177" s="1" t="s">
@@ -2761,7 +2779,7 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="B178" s="1" t="s">
@@ -2773,7 +2791,7 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="B179" s="1" t="s">
@@ -2785,7 +2803,7 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="B180" s="1" t="s">
@@ -2797,7 +2815,7 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="B181" s="1" t="s">
@@ -2809,7 +2827,7 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="B182" s="1" t="s">
@@ -2848,7 +2866,7 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185">
-        <f t="shared" ref="A185:A202" si="10">A184</f>
+        <f t="shared" ref="A185:A202" si="11">A184</f>
         <v>7</v>
       </c>
       <c r="B185" s="1" t="s">
@@ -2860,7 +2878,7 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="B186" s="1" t="s">
@@ -2872,7 +2890,7 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="B187" s="1" t="s">
@@ -2884,7 +2902,7 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="B188" s="1" t="s">
@@ -2896,7 +2914,7 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="B189" s="1" t="s">
@@ -2908,7 +2926,7 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="B190" s="1" t="s">
@@ -2920,7 +2938,7 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="B191" s="1" t="s">
@@ -2932,7 +2950,7 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="B192" s="1" t="s">
@@ -2944,7 +2962,7 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="B193" s="1" t="s">
@@ -2956,7 +2974,7 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="B194" s="1" t="s">
@@ -2968,7 +2986,7 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="B195" s="1" t="s">
@@ -2980,7 +2998,7 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="B196" s="1" t="s">
@@ -2992,7 +3010,7 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="B197" s="1" t="s">
@@ -3004,7 +3022,7 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="B198" s="1" t="s">
@@ -3016,7 +3034,7 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="B199" s="1" t="s">
@@ -3028,7 +3046,7 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="B200" s="1" t="s">
@@ -3040,7 +3058,7 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="B201" s="1" t="s">
@@ -3052,7 +3070,7 @@
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="B202" s="1" t="s">
@@ -3064,7 +3082,7 @@
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203">
-        <f>A187</f>
+        <f t="shared" ref="A203:A213" si="12">A187</f>
         <v>7</v>
       </c>
       <c r="B203" s="1" t="s">
@@ -3076,7 +3094,7 @@
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204">
-        <f>A188</f>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="B204" s="1" t="s">
@@ -3088,7 +3106,7 @@
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205">
-        <f>A189</f>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="B205" s="1" t="s">
@@ -3100,7 +3118,7 @@
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206">
-        <f>A190</f>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="B206" s="1" t="s">
@@ -3112,7 +3130,7 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207">
-        <f>A191</f>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="B207" s="1" t="s">
@@ -3124,7 +3142,7 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A208">
-        <f>A192</f>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="B208" s="1" t="s">
@@ -3136,7 +3154,7 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209">
-        <f>A193</f>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="B209" s="1" t="s">
@@ -3148,7 +3166,7 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210">
-        <f>A194</f>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="B210" s="1" t="s">
@@ -3160,7 +3178,7 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211">
-        <f>A195</f>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="B211" s="1" t="s">
@@ -3172,7 +3190,7 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212">
-        <f>A196</f>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="B212" s="1" t="s">
@@ -3184,7 +3202,7 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213">
-        <f>A197</f>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="B213" s="1" t="s">
@@ -3196,7 +3214,7 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214">
-        <f t="shared" ref="A214:A222" si="11">A203</f>
+        <f t="shared" ref="A214:A222" si="13">A203</f>
         <v>7</v>
       </c>
       <c r="B214" s="1" t="s">
@@ -3208,7 +3226,7 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>7</v>
       </c>
       <c r="B215" s="1" t="s">
@@ -3220,7 +3238,7 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>7</v>
       </c>
       <c r="B216" s="1" t="s">
@@ -3232,7 +3250,7 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>7</v>
       </c>
       <c r="B217" s="1" t="s">
@@ -3244,7 +3262,7 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>7</v>
       </c>
       <c r="B218" s="1" t="s">
@@ -3256,7 +3274,7 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>7</v>
       </c>
       <c r="B219" s="1" t="s">
@@ -3268,7 +3286,7 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>7</v>
       </c>
       <c r="B220" s="1" t="s">
@@ -3280,7 +3298,7 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>7</v>
       </c>
       <c r="B221" s="1" t="s">
@@ -3292,7 +3310,7 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>7</v>
       </c>
       <c r="B222" s="1" t="s">
@@ -3331,7 +3349,7 @@
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A225">
-        <f t="shared" ref="A225:A242" si="12">A224</f>
+        <f t="shared" ref="A225:A242" si="14">A224</f>
         <v>8</v>
       </c>
       <c r="B225" s="1" t="s">
@@ -3343,7 +3361,7 @@
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="B226" s="1" t="s">
@@ -3355,7 +3373,7 @@
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="B227" s="1" t="s">
@@ -3367,7 +3385,7 @@
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="B228" s="1" t="s">
@@ -3379,7 +3397,7 @@
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A229">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="B229" s="1" t="s">
@@ -3391,7 +3409,7 @@
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A230">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="B230" s="1" t="s">
@@ -3403,7 +3421,7 @@
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A231">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="B231" s="1" t="s">
@@ -3415,7 +3433,7 @@
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="B232" s="1" t="s">
@@ -3427,7 +3445,7 @@
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A233">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="B233" s="1" t="s">
@@ -3439,7 +3457,7 @@
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A234">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="B234" s="1" t="s">
@@ -3451,7 +3469,7 @@
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A235">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="B235" s="1" t="s">
@@ -3463,7 +3481,7 @@
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A236">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="B236" s="1" t="s">
@@ -3475,7 +3493,7 @@
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A237">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="B237" s="1" t="s">
@@ -3487,7 +3505,7 @@
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A238">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="B238" s="1" t="s">
@@ -3499,7 +3517,7 @@
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A239">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="B239" s="1" t="s">
@@ -3511,7 +3529,7 @@
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A240">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="B240" s="1" t="s">
@@ -3523,7 +3541,7 @@
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A241">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="B241" s="1" t="s">
@@ -3535,7 +3553,7 @@
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A242">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="B242" s="1" t="s">
@@ -3547,7 +3565,7 @@
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A243">
-        <f>A227</f>
+        <f t="shared" ref="A243:A253" si="15">A227</f>
         <v>8</v>
       </c>
       <c r="B243" s="1" t="s">
@@ -3559,7 +3577,7 @@
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A244">
-        <f>A228</f>
+        <f t="shared" si="15"/>
         <v>8</v>
       </c>
       <c r="B244" s="1" t="s">
@@ -3571,7 +3589,7 @@
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A245">
-        <f>A229</f>
+        <f t="shared" si="15"/>
         <v>8</v>
       </c>
       <c r="B245" s="1" t="s">
@@ -3583,7 +3601,7 @@
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A246">
-        <f>A230</f>
+        <f t="shared" si="15"/>
         <v>8</v>
       </c>
       <c r="B246" s="1" t="s">
@@ -3595,7 +3613,7 @@
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A247">
-        <f>A231</f>
+        <f t="shared" si="15"/>
         <v>8</v>
       </c>
       <c r="B247" s="1" t="s">
@@ -3607,7 +3625,7 @@
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A248">
-        <f>A232</f>
+        <f t="shared" si="15"/>
         <v>8</v>
       </c>
       <c r="B248" s="1" t="s">
@@ -3619,7 +3637,7 @@
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A249">
-        <f>A233</f>
+        <f t="shared" si="15"/>
         <v>8</v>
       </c>
       <c r="B249" s="1" t="s">
@@ -3631,7 +3649,7 @@
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A250">
-        <f>A234</f>
+        <f t="shared" si="15"/>
         <v>8</v>
       </c>
       <c r="B250" s="1" t="s">
@@ -3643,7 +3661,7 @@
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A251">
-        <f>A235</f>
+        <f t="shared" si="15"/>
         <v>8</v>
       </c>
       <c r="B251" s="1" t="s">
@@ -3655,7 +3673,7 @@
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A252">
-        <f>A236</f>
+        <f t="shared" si="15"/>
         <v>8</v>
       </c>
       <c r="B252" s="1" t="s">
@@ -3667,7 +3685,7 @@
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A253">
-        <f>A237</f>
+        <f t="shared" si="15"/>
         <v>8</v>
       </c>
       <c r="B253" s="1" t="s">
@@ -3679,7 +3697,7 @@
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A254">
-        <f t="shared" ref="A254:A262" si="13">A243</f>
+        <f t="shared" ref="A254:A262" si="16">A243</f>
         <v>8</v>
       </c>
       <c r="B254" s="1" t="s">
@@ -3691,7 +3709,7 @@
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A255">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="B255" s="1" t="s">
@@ -3703,7 +3721,7 @@
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A256">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="B256" s="1" t="s">
@@ -3715,7 +3733,7 @@
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A257">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="B257" s="1" t="s">
@@ -3727,7 +3745,7 @@
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A258">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="B258" s="1" t="s">
@@ -3739,7 +3757,7 @@
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A259">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="B259" s="1" t="s">
@@ -3751,7 +3769,7 @@
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A260">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="B260" s="1" t="s">
@@ -3763,7 +3781,7 @@
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A261">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="B261" s="1" t="s">
@@ -3775,7 +3793,7 @@
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A262">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="B262" s="1" t="s">
@@ -3814,7 +3832,7 @@
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A265">
-        <f t="shared" ref="A265:A287" si="14">A264</f>
+        <f t="shared" ref="A265:A287" si="17">A264</f>
         <v>9</v>
       </c>
       <c r="B265" s="1" t="s">
@@ -3826,7 +3844,7 @@
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A266">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
       <c r="B266" s="1" t="s">
@@ -3838,7 +3856,7 @@
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A267">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
       <c r="B267" s="1" t="s">
@@ -3850,7 +3868,7 @@
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A268">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
       <c r="B268" s="1" t="s">
@@ -3862,7 +3880,7 @@
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A269">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
       <c r="B269" s="1" t="s">
@@ -3874,7 +3892,7 @@
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A270">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
       <c r="B270" s="1" t="s">
@@ -3886,7 +3904,7 @@
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A271">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
       <c r="B271" s="1" t="s">
@@ -3898,7 +3916,7 @@
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A272">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
       <c r="B272" s="1" t="s">
@@ -3910,7 +3928,7 @@
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A273">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
       <c r="B273" s="1" t="s">
@@ -3922,7 +3940,7 @@
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A274">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
       <c r="B274" s="1" t="s">
@@ -3934,7 +3952,7 @@
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A275">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
       <c r="B275" s="1" t="s">
@@ -3946,7 +3964,7 @@
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A276">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
       <c r="B276" s="1" t="s">
@@ -3958,7 +3976,7 @@
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A277">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
       <c r="B277" s="1" t="s">
@@ -3970,7 +3988,7 @@
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A278">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
       <c r="B278" s="1" t="s">
@@ -3982,7 +4000,7 @@
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A279">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
       <c r="B279" s="1" t="s">
@@ -3994,7 +4012,7 @@
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A280">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
       <c r="B280" s="1" t="s">
@@ -4006,7 +4024,7 @@
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A281">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
       <c r="B281" s="1" t="s">
@@ -4018,7 +4036,7 @@
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A282">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
       <c r="B282" s="1" t="s">
@@ -4030,7 +4048,7 @@
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A283">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
       <c r="B283" s="1" t="s">
@@ -4042,7 +4060,7 @@
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A284">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
       <c r="B284" s="1" t="s">
@@ -4054,7 +4072,7 @@
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A285">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
       <c r="B285" s="1" t="s">
@@ -4066,7 +4084,7 @@
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A286">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
       <c r="B286" s="1" t="s">
@@ -4078,7 +4096,7 @@
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A287">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
       <c r="B287" s="1" t="s">
@@ -4090,7 +4108,7 @@
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A288">
-        <f>A267</f>
+        <f t="shared" ref="A288:A298" si="18">A267</f>
         <v>9</v>
       </c>
       <c r="B288" s="1" t="s">
@@ -4102,7 +4120,7 @@
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A289">
-        <f>A268</f>
+        <f t="shared" si="18"/>
         <v>9</v>
       </c>
       <c r="B289" s="1" t="s">
@@ -4114,7 +4132,7 @@
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A290">
-        <f>A269</f>
+        <f t="shared" si="18"/>
         <v>9</v>
       </c>
       <c r="B290" s="1" t="s">
@@ -4126,7 +4144,7 @@
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A291">
-        <f>A270</f>
+        <f t="shared" si="18"/>
         <v>9</v>
       </c>
       <c r="B291" s="1" t="s">
@@ -4138,7 +4156,7 @@
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A292">
-        <f>A271</f>
+        <f t="shared" si="18"/>
         <v>9</v>
       </c>
       <c r="B292" s="1" t="s">
@@ -4150,7 +4168,7 @@
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A293">
-        <f>A272</f>
+        <f t="shared" si="18"/>
         <v>9</v>
       </c>
       <c r="B293" s="1" t="s">
@@ -4162,7 +4180,7 @@
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A294">
-        <f>A273</f>
+        <f t="shared" si="18"/>
         <v>9</v>
       </c>
       <c r="B294" s="1" t="s">
@@ -4174,7 +4192,7 @@
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A295">
-        <f>A274</f>
+        <f t="shared" si="18"/>
         <v>9</v>
       </c>
       <c r="B295" s="1" t="s">
@@ -4186,7 +4204,7 @@
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A296">
-        <f>A275</f>
+        <f t="shared" si="18"/>
         <v>9</v>
       </c>
       <c r="B296" s="1" t="s">
@@ -4198,7 +4216,7 @@
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A297">
-        <f>A276</f>
+        <f t="shared" si="18"/>
         <v>9</v>
       </c>
       <c r="B297" s="1" t="s">
@@ -4210,7 +4228,7 @@
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A298">
-        <f>A277</f>
+        <f t="shared" si="18"/>
         <v>9</v>
       </c>
       <c r="B298" s="1" t="s">
@@ -4222,7 +4240,7 @@
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A299">
-        <f t="shared" ref="A299:A312" si="15">A288</f>
+        <f t="shared" ref="A299:A312" si="19">A288</f>
         <v>9</v>
       </c>
       <c r="B299" s="1" t="s">
@@ -4234,7 +4252,7 @@
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A300">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>9</v>
       </c>
       <c r="B300" s="1" t="s">
@@ -4246,7 +4264,7 @@
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A301">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>9</v>
       </c>
       <c r="B301" s="1" t="s">
@@ -4258,7 +4276,7 @@
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A302">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>9</v>
       </c>
       <c r="B302" s="1" t="s">
@@ -4270,7 +4288,7 @@
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A303">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>9</v>
       </c>
       <c r="B303" s="1" t="s">
@@ -4282,7 +4300,7 @@
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A304">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>9</v>
       </c>
       <c r="B304" s="1" t="s">
@@ -4294,7 +4312,7 @@
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A305">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>9</v>
       </c>
       <c r="B305" s="1" t="s">
@@ -4306,7 +4324,7 @@
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A306">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>9</v>
       </c>
       <c r="B306" s="1" t="s">
@@ -4318,7 +4336,7 @@
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A307">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>9</v>
       </c>
       <c r="B307" s="1" t="s">
@@ -4330,7 +4348,7 @@
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A308">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>9</v>
       </c>
       <c r="B308" s="1" t="s">
@@ -4342,7 +4360,7 @@
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A309">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>9</v>
       </c>
       <c r="B309" s="1" t="s">
@@ -4354,7 +4372,7 @@
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A310">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>9</v>
       </c>
       <c r="B310" s="1" t="s">
@@ -4366,7 +4384,7 @@
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A311">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>9</v>
       </c>
       <c r="B311" s="1" t="s">
@@ -4378,7 +4396,7 @@
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A312">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>9</v>
       </c>
       <c r="B312" s="1" t="s">
@@ -4417,7 +4435,7 @@
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A315">
-        <f t="shared" ref="A315:A337" si="16">A314</f>
+        <f t="shared" ref="A315:A337" si="20">A314</f>
         <v>10</v>
       </c>
       <c r="B315" s="1" t="s">
@@ -4429,7 +4447,7 @@
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A316">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>10</v>
       </c>
       <c r="B316" s="1" t="s">
@@ -4441,7 +4459,7 @@
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A317">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>10</v>
       </c>
       <c r="B317" s="1" t="s">
@@ -4453,7 +4471,7 @@
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A318">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>10</v>
       </c>
       <c r="B318" s="1" t="s">
@@ -4465,7 +4483,7 @@
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A319">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>10</v>
       </c>
       <c r="B319" s="1" t="s">
@@ -4477,7 +4495,7 @@
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A320">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>10</v>
       </c>
       <c r="B320" s="1" t="s">
@@ -4489,7 +4507,7 @@
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A321">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>10</v>
       </c>
       <c r="B321" s="1" t="s">
@@ -4501,7 +4519,7 @@
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A322">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>10</v>
       </c>
       <c r="B322" s="1" t="s">
@@ -4513,7 +4531,7 @@
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A323">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>10</v>
       </c>
       <c r="B323" s="1" t="s">
@@ -4525,7 +4543,7 @@
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A324">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>10</v>
       </c>
       <c r="B324" s="1" t="s">
@@ -4537,7 +4555,7 @@
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A325">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>10</v>
       </c>
       <c r="B325" s="1" t="s">
@@ -4549,7 +4567,7 @@
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A326">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>10</v>
       </c>
       <c r="B326" s="1" t="s">
@@ -4561,7 +4579,7 @@
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A327">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>10</v>
       </c>
       <c r="B327" s="1" t="s">
@@ -4573,7 +4591,7 @@
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A328">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>10</v>
       </c>
       <c r="B328" s="1" t="s">
@@ -4585,7 +4603,7 @@
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A329">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>10</v>
       </c>
       <c r="B329" s="1" t="s">
@@ -4597,7 +4615,7 @@
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A330">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>10</v>
       </c>
       <c r="B330" s="1" t="s">
@@ -4609,7 +4627,7 @@
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A331">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>10</v>
       </c>
       <c r="B331" s="1" t="s">
@@ -4621,7 +4639,7 @@
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A332">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>10</v>
       </c>
       <c r="B332" s="1" t="s">
@@ -4633,7 +4651,7 @@
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A333">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>10</v>
       </c>
       <c r="B333" s="1" t="s">
@@ -4645,7 +4663,7 @@
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A334">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>10</v>
       </c>
       <c r="B334" s="1" t="s">
@@ -4657,7 +4675,7 @@
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A335">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>10</v>
       </c>
       <c r="B335" s="1" t="s">
@@ -4669,7 +4687,7 @@
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A336">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>10</v>
       </c>
       <c r="B336" s="1" t="s">
@@ -4681,7 +4699,7 @@
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A337">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>10</v>
       </c>
       <c r="B337" s="1" t="s">
@@ -4693,7 +4711,7 @@
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A338">
-        <f>A317</f>
+        <f t="shared" ref="A338:A348" si="21">A317</f>
         <v>10</v>
       </c>
       <c r="B338" s="1" t="s">
@@ -4705,7 +4723,7 @@
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A339">
-        <f>A318</f>
+        <f t="shared" si="21"/>
         <v>10</v>
       </c>
       <c r="B339" s="1" t="s">
@@ -4717,7 +4735,7 @@
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A340">
-        <f>A319</f>
+        <f t="shared" si="21"/>
         <v>10</v>
       </c>
       <c r="B340" s="1" t="s">
@@ -4729,7 +4747,7 @@
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A341">
-        <f>A320</f>
+        <f t="shared" si="21"/>
         <v>10</v>
       </c>
       <c r="B341" s="1" t="s">
@@ -4741,7 +4759,7 @@
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A342">
-        <f>A321</f>
+        <f t="shared" si="21"/>
         <v>10</v>
       </c>
       <c r="B342" s="1" t="s">
@@ -4753,7 +4771,7 @@
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A343">
-        <f>A322</f>
+        <f t="shared" si="21"/>
         <v>10</v>
       </c>
       <c r="B343" s="1" t="s">
@@ -4765,7 +4783,7 @@
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A344">
-        <f>A323</f>
+        <f t="shared" si="21"/>
         <v>10</v>
       </c>
       <c r="B344" s="1" t="s">
@@ -4777,7 +4795,7 @@
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A345">
-        <f>A324</f>
+        <f t="shared" si="21"/>
         <v>10</v>
       </c>
       <c r="B345" s="1" t="s">
@@ -4789,7 +4807,7 @@
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A346">
-        <f>A325</f>
+        <f t="shared" si="21"/>
         <v>10</v>
       </c>
       <c r="B346" s="1" t="s">
@@ -4801,7 +4819,7 @@
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A347">
-        <f>A326</f>
+        <f t="shared" si="21"/>
         <v>10</v>
       </c>
       <c r="B347" s="1" t="s">
@@ -4813,7 +4831,7 @@
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A348">
-        <f>A327</f>
+        <f t="shared" si="21"/>
         <v>10</v>
       </c>
       <c r="B348" s="1" t="s">
@@ -4825,7 +4843,7 @@
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A349">
-        <f t="shared" ref="A349:A362" si="17">A338</f>
+        <f t="shared" ref="A349:A362" si="22">A338</f>
         <v>10</v>
       </c>
       <c r="B349" s="1" t="s">
@@ -4837,7 +4855,7 @@
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A350">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>10</v>
       </c>
       <c r="B350" s="1" t="s">
@@ -4849,7 +4867,7 @@
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A351">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>10</v>
       </c>
       <c r="B351" s="1" t="s">
@@ -4861,7 +4879,7 @@
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A352">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>10</v>
       </c>
       <c r="B352" s="1" t="s">
@@ -4873,7 +4891,7 @@
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A353">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>10</v>
       </c>
       <c r="B353" s="1" t="s">
@@ -4885,7 +4903,7 @@
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A354">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>10</v>
       </c>
       <c r="B354" s="1" t="s">
@@ -4897,7 +4915,7 @@
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A355">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>10</v>
       </c>
       <c r="B355" s="1" t="s">
@@ -4909,7 +4927,7 @@
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A356">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>10</v>
       </c>
       <c r="B356" s="1" t="s">
@@ -4921,7 +4939,7 @@
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A357">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>10</v>
       </c>
       <c r="B357" s="1" t="s">
@@ -4933,7 +4951,7 @@
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A358">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>10</v>
       </c>
       <c r="B358" s="1" t="s">
@@ -4945,7 +4963,7 @@
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A359">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>10</v>
       </c>
       <c r="B359" s="1" t="s">
@@ -4957,7 +4975,7 @@
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A360">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>10</v>
       </c>
       <c r="B360" s="1" t="s">
@@ -4969,7 +4987,7 @@
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A361">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>10</v>
       </c>
       <c r="B361" s="1" t="s">
@@ -4981,7 +4999,7 @@
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A362">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>10</v>
       </c>
       <c r="B362" s="1" t="s">
@@ -5007,10 +5025,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E6FFAFD-B9D4-4D16-9C10-FE1E60CA3279}">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:C122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5020,12 +5038,12 @@
     <col min="3" max="3" width="19.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -5036,7 +5054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -5044,10 +5062,10 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>1112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>A3</f>
         <v>1</v>
@@ -5056,22 +5074,22 @@
         <v>11</v>
       </c>
       <c r="C4">
-        <v>1111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f t="shared" ref="A5:A11" si="0">A4</f>
+        <f t="shared" ref="A5:A17" si="0">A4</f>
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C5">
-        <v>1111</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -5080,10 +5098,10 @@
         <v>13</v>
       </c>
       <c r="C6">
-        <v>1111</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -5092,336 +5110,303 @@
         <v>14</v>
       </c>
       <c r="C7">
-        <v>1111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C8">
-        <v>1111</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>198000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>A8</f>
+        <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C9">
-        <v>1111</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>198000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C10">
-        <v>1111</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>198000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>198000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>198000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C11">
-        <v>1111</v>
-      </c>
-      <c r="G11">
-        <f>SUM(C3:C11)</f>
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>2</v>
-      </c>
-      <c r="B12" s="1" t="str">
-        <f>B3</f>
-        <v>S0001</v>
-      </c>
-      <c r="C12">
-        <f>C3</f>
-        <v>1112</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <f>A12</f>
-        <v>2</v>
-      </c>
-      <c r="B13" s="1" t="str">
-        <f>B4</f>
-        <v>S0002</v>
-      </c>
-      <c r="C13">
-        <f t="shared" ref="C13:C47" si="1">C4</f>
-        <v>1111</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <f t="shared" ref="A14:A20" si="2">A13</f>
-        <v>2</v>
-      </c>
-      <c r="B14" s="1" t="str">
-        <f>B5</f>
-        <v>S0003</v>
-      </c>
-      <c r="C14">
-        <f t="shared" si="1"/>
-        <v>1111</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="B15" s="1" t="str">
-        <f>B6</f>
-        <v>S0004</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="1"/>
-        <v>1111</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="B16" s="1" t="str">
-        <f>B7</f>
-        <v>S0005</v>
-      </c>
       <c r="C16">
-        <f t="shared" si="1"/>
-        <v>1111</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="B17" s="1" t="str">
-        <f>B8</f>
-        <v>S0006</v>
+      <c r="B17" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C17">
-        <f t="shared" si="1"/>
-        <v>1111</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="B18" s="1" t="str">
-        <f t="shared" ref="B18:B47" si="3">B9</f>
-        <v>S0007</v>
+        <v>3</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C18">
-        <f t="shared" si="1"/>
-        <v>1111</v>
+        <v>196000</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="B19" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>S0008</v>
+        <f>A18</f>
+        <v>3</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C19">
-        <f t="shared" si="1"/>
-        <v>1111</v>
+        <f>C18</f>
+        <v>196000</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="B20" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>S0009</v>
+        <f t="shared" ref="A20:A27" si="1">A19</f>
+        <v>3</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C20">
-        <f t="shared" si="1"/>
-        <v>1111</v>
+        <f t="shared" ref="C20:C22" si="2">C19</f>
+        <v>196000</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B21" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>S0001</v>
+      <c r="B21" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C21">
-        <f t="shared" si="1"/>
-        <v>1112</v>
+        <f t="shared" si="2"/>
+        <v>196000</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
-        <f t="shared" ref="A22:A38" si="4">A21</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B22" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>S0002</v>
+      <c r="B22" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C22">
-        <f t="shared" si="1"/>
-        <v>1111</v>
+        <f t="shared" si="2"/>
+        <v>196000</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B23" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>S0003</v>
+      <c r="B23" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C23">
-        <f t="shared" si="1"/>
-        <v>1111</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B24" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>S0004</v>
+      <c r="B24" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C24">
-        <f t="shared" si="1"/>
-        <v>1111</v>
+        <f>C23</f>
+        <v>4000</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B25" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>S0005</v>
+      <c r="B25" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C25">
-        <f t="shared" si="1"/>
-        <v>1111</v>
+        <f t="shared" ref="C25:C27" si="3">C24</f>
+        <v>4000</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B26" s="1" t="str">
+      <c r="B26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26">
         <f t="shared" si="3"/>
-        <v>S0006</v>
-      </c>
-      <c r="C26">
-        <f t="shared" si="1"/>
-        <v>1111</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B27" s="1" t="str">
+      <c r="B27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27">
         <f t="shared" si="3"/>
-        <v>S0007</v>
-      </c>
-      <c r="C27">
-        <f t="shared" si="1"/>
-        <v>1111</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="B28" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>S0008</v>
+        <v>4</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C28">
-        <f t="shared" si="1"/>
-        <v>1111</v>
+        <v>193000</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="B29" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>S0009</v>
+        <f>A28</f>
+        <v>4</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C29">
-        <f t="shared" si="1"/>
-        <v>1111</v>
+        <f>C28</f>
+        <v>193000</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
+        <f t="shared" ref="A30:A37" si="4">A29</f>
         <v>4</v>
       </c>
-      <c r="B30" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>S0001</v>
+      <c r="B30" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C30">
-        <f t="shared" si="1"/>
-        <v>1112</v>
+        <f t="shared" ref="C30:C32" si="5">C29</f>
+        <v>193000</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
-        <f t="shared" ref="A31" si="5">A30</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="B31" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>S0002</v>
+      <c r="B31" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C31">
-        <f t="shared" si="1"/>
-        <v>1111</v>
+        <f t="shared" si="5"/>
+        <v>193000</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -5429,13 +5414,12 @@
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="B32" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>S0003</v>
+      <c r="B32" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C32">
-        <f t="shared" si="1"/>
-        <v>1111</v>
+        <f t="shared" si="5"/>
+        <v>193000</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -5443,13 +5427,11 @@
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="B33" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>S0004</v>
+      <c r="B33" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C33">
-        <f t="shared" si="1"/>
-        <v>1111</v>
+        <v>7000</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -5457,13 +5439,12 @@
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="B34" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>S0005</v>
+      <c r="B34" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C34">
-        <f t="shared" si="1"/>
-        <v>1111</v>
+        <f>C33</f>
+        <v>7000</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -5471,13 +5452,12 @@
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="B35" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>S0006</v>
+      <c r="B35" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C35">
-        <f t="shared" si="1"/>
-        <v>1111</v>
+        <f t="shared" ref="C35:C37" si="6">C34</f>
+        <v>7000</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -5485,13 +5465,12 @@
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="B36" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>S0007</v>
+      <c r="B36" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="C36">
-        <f t="shared" si="1"/>
-        <v>1111</v>
+        <f t="shared" si="6"/>
+        <v>7000</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -5499,152 +5478,1094 @@
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="B37" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>S0008</v>
+      <c r="B37" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C37">
-        <f t="shared" si="1"/>
-        <v>1111</v>
+        <f t="shared" si="6"/>
+        <v>7000</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="B38" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>S0009</v>
+        <v>5</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C38">
-        <f t="shared" si="1"/>
-        <v>1111</v>
+        <v>190000</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
+        <f>A38</f>
         <v>5</v>
       </c>
-      <c r="B39" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>S0001</v>
+      <c r="B39" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C39">
-        <f t="shared" si="1"/>
-        <v>1112</v>
+        <f>C38</f>
+        <v>190000</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
-        <f t="shared" ref="A40:A47" si="6">A39</f>
+        <f t="shared" ref="A40:A62" si="7">A39</f>
         <v>5</v>
       </c>
-      <c r="B40" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>S0002</v>
+      <c r="B40" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C40">
-        <f t="shared" si="1"/>
-        <v>1111</v>
+        <f t="shared" ref="C40:C42" si="8">C39</f>
+        <v>190000</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
-      <c r="B41" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>S0003</v>
+      <c r="B41" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C41">
-        <f t="shared" si="1"/>
-        <v>1111</v>
+        <f t="shared" si="8"/>
+        <v>190000</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
-      <c r="B42" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>S0004</v>
+      <c r="B42" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C42">
-        <f t="shared" si="1"/>
-        <v>1111</v>
+        <f t="shared" si="8"/>
+        <v>190000</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
-      <c r="B43" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>S0005</v>
+      <c r="B43" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C43">
-        <f t="shared" si="1"/>
-        <v>1111</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
-      <c r="B44" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>S0006</v>
+      <c r="B44" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C44">
-        <f t="shared" si="1"/>
-        <v>1111</v>
+        <f>C43</f>
+        <v>10000</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
-      <c r="B45" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>S0007</v>
+      <c r="B45" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C45">
-        <f t="shared" si="1"/>
-        <v>1111</v>
+        <f t="shared" ref="C45:C47" si="9">C44</f>
+        <v>10000</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
-      <c r="B46" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>S0008</v>
+      <c r="B46" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="C46">
-        <f t="shared" si="1"/>
-        <v>1111</v>
+        <f t="shared" si="9"/>
+        <v>10000</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
-      <c r="B47" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>S0009</v>
+      <c r="B47" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C47">
-        <f t="shared" si="1"/>
-        <v>1111</v>
+        <f t="shared" si="9"/>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>6</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48">
+        <v>184900</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <f>A48</f>
+        <v>6</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49">
+        <f>C48</f>
+        <v>184900</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C50">
+        <f t="shared" ref="C50:C52" si="10">C49</f>
+        <v>184900</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="10"/>
+        <v>184900</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="10"/>
+        <v>184900</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C53">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C54">
+        <f>C53</f>
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C55">
+        <f t="shared" ref="C55:C57" si="11">C54</f>
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="11"/>
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="11"/>
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C58">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C59">
+        <f>C58</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C60">
+        <f t="shared" ref="C60:C62" si="12">C59</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="12"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="12"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>7</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C63">
+        <v>179800</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <f>A63</f>
+        <v>7</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C64">
+        <f>C63</f>
+        <v>179800</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <f t="shared" ref="A65:A77" si="13">A64</f>
+        <v>7</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C65">
+        <f t="shared" ref="C65:C67" si="14">C64</f>
+        <v>179800</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <f t="shared" si="13"/>
+        <v>7</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="14"/>
+        <v>179800</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <f t="shared" si="13"/>
+        <v>7</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="14"/>
+        <v>179800</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <f t="shared" si="13"/>
+        <v>7</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C68">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <f t="shared" si="13"/>
+        <v>7</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C69">
+        <f>C68</f>
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <f t="shared" si="13"/>
+        <v>7</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C70">
+        <f t="shared" ref="C70:C72" si="15">C69</f>
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <f t="shared" si="13"/>
+        <v>7</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C71">
+        <f t="shared" si="15"/>
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <f t="shared" si="13"/>
+        <v>7</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C72">
+        <f t="shared" si="15"/>
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <f t="shared" si="13"/>
+        <v>7</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C73">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <f t="shared" si="13"/>
+        <v>7</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C74">
+        <f>C73</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <f t="shared" si="13"/>
+        <v>7</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C75">
+        <f t="shared" ref="C75:C77" si="16">C74</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <f t="shared" si="13"/>
+        <v>7</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="16"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <f t="shared" si="13"/>
+        <v>7</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="16"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>8</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C78">
+        <v>169200</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <f>A78</f>
+        <v>8</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C79">
+        <f>C78</f>
+        <v>169200</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <f t="shared" ref="A80:A92" si="17">A79</f>
+        <v>8</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C80">
+        <f t="shared" ref="C80:C82" si="18">C79</f>
+        <v>169200</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C81">
+        <f t="shared" si="18"/>
+        <v>169200</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C82">
+        <f t="shared" si="18"/>
+        <v>169200</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C83">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C84">
+        <f>C83</f>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C85">
+        <f t="shared" ref="C85:C87" si="19">C84</f>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C86">
+        <f t="shared" si="19"/>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C87">
+        <f t="shared" si="19"/>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C88">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C89">
+        <f>C88</f>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C90">
+        <f t="shared" ref="C90:C92" si="20">C89</f>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C91">
+        <f t="shared" si="20"/>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C92">
+        <f t="shared" si="20"/>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>9</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C93">
+        <v>158600</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <f>A93</f>
+        <v>9</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C94">
+        <f>C93</f>
+        <v>158600</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <f t="shared" ref="A95:A107" si="21">A94</f>
+        <v>9</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C95">
+        <f t="shared" ref="C95:C97" si="22">C94</f>
+        <v>158600</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C96">
+        <f t="shared" si="22"/>
+        <v>158600</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C97">
+        <f t="shared" si="22"/>
+        <v>158600</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C98">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C99">
+        <f>C98</f>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C100">
+        <f t="shared" ref="C100:C102" si="23">C99</f>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C101">
+        <f t="shared" si="23"/>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C102">
+        <f t="shared" si="23"/>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C103">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C104">
+        <f>C103</f>
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C105">
+        <f t="shared" ref="C105:C107" si="24">C104</f>
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C106">
+        <f t="shared" si="24"/>
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C107">
+        <f t="shared" si="24"/>
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>10</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C108">
+        <v>138000</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <f>A108</f>
+        <v>10</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C109">
+        <f>C108</f>
+        <v>138000</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <f t="shared" ref="A110:A122" si="25">A109</f>
+        <v>10</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C110">
+        <f t="shared" ref="C110:C112" si="26">C109</f>
+        <v>138000</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <f t="shared" si="25"/>
+        <v>10</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C111">
+        <f t="shared" si="26"/>
+        <v>138000</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <f t="shared" si="25"/>
+        <v>10</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C112">
+        <f t="shared" si="26"/>
+        <v>138000</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <f t="shared" si="25"/>
+        <v>10</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C113">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <f t="shared" si="25"/>
+        <v>10</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C114">
+        <f>C113</f>
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <f t="shared" si="25"/>
+        <v>10</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C115">
+        <f t="shared" ref="C115:C117" si="27">C114</f>
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <f t="shared" si="25"/>
+        <v>10</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C116">
+        <f t="shared" si="27"/>
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <f t="shared" si="25"/>
+        <v>10</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C117">
+        <f t="shared" si="27"/>
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A118">
+        <f t="shared" si="25"/>
+        <v>10</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C118">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <f t="shared" si="25"/>
+        <v>10</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C119">
+        <f>C118</f>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <f t="shared" si="25"/>
+        <v>10</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C120">
+        <f t="shared" ref="C120:C122" si="28">C119</f>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A121">
+        <f t="shared" si="25"/>
+        <v>10</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C121">
+        <f t="shared" si="28"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122">
+        <f t="shared" si="25"/>
+        <v>10</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C122">
+        <f t="shared" si="28"/>
+        <v>2000</v>
       </c>
     </row>
   </sheetData>
@@ -5659,10 +6580,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF1FBEA-E97D-46D7-B77D-7F9DD3257CDE}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5696,7 +6617,7 @@
         <v>21</v>
       </c>
       <c r="C3">
-        <v>1666</v>
+        <v>333334</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -5708,7 +6629,7 @@
         <v>22</v>
       </c>
       <c r="C4">
-        <v>1666</v>
+        <v>333333</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -5720,7 +6641,7 @@
         <v>23</v>
       </c>
       <c r="C5">
-        <v>1667</v>
+        <v>333333</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -5732,7 +6653,7 @@
         <v>24</v>
       </c>
       <c r="C6">
-        <v>1667</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -5744,7 +6665,7 @@
         <v>25</v>
       </c>
       <c r="C7">
-        <v>1667</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -5756,11 +6677,11 @@
         <v>26</v>
       </c>
       <c r="C8">
-        <v>1667</v>
+        <v>0</v>
       </c>
       <c r="D8">
         <f>SUM(C3:C8)</f>
-        <v>10000</v>
+        <v>1000000</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -5772,8 +6693,7 @@
         <v>F0001</v>
       </c>
       <c r="C9">
-        <f>C3</f>
-        <v>1666</v>
+        <v>330001</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -5786,13 +6706,12 @@
         <v>F0002</v>
       </c>
       <c r="C10">
-        <f t="shared" ref="C10:C32" si="1">C4</f>
-        <v>1666</v>
+        <v>330000</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
-        <f t="shared" ref="A11:A14" si="2">A10</f>
+        <f t="shared" ref="A11:A14" si="1">A10</f>
         <v>2</v>
       </c>
       <c r="B11" s="1" t="str">
@@ -5800,13 +6719,12 @@
         <v>F0003</v>
       </c>
       <c r="C11">
-        <f t="shared" si="1"/>
-        <v>1667</v>
+        <v>330000</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="B12" s="1" t="str">
@@ -5814,13 +6732,12 @@
         <v>F0004</v>
       </c>
       <c r="C12">
-        <f t="shared" si="1"/>
-        <v>1667</v>
+        <v>3333</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="B13" s="1" t="str">
@@ -5828,13 +6745,12 @@
         <v>F0005</v>
       </c>
       <c r="C13">
-        <f t="shared" si="1"/>
-        <v>1667</v>
+        <v>3333</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="B14" s="1" t="str">
@@ -5842,8 +6758,11 @@
         <v>F0006</v>
       </c>
       <c r="C14">
-        <f t="shared" si="1"/>
-        <v>1667</v>
+        <v>3333</v>
+      </c>
+      <c r="D14">
+        <f>SUM(C9:C14)</f>
+        <v>1000000</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -5851,86 +6770,80 @@
         <v>3</v>
       </c>
       <c r="B15" s="1" t="str">
-        <f t="shared" ref="B15:B32" si="3">B9</f>
+        <f t="shared" ref="B15:B62" si="2">B9</f>
         <v>F0001</v>
       </c>
       <c r="C15">
-        <f t="shared" si="1"/>
-        <v>1666</v>
+        <v>326668</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
-        <f t="shared" ref="A16:A32" si="4">A15</f>
+        <f t="shared" ref="A16:A32" si="3">A15</f>
         <v>3</v>
       </c>
       <c r="B16" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>F0002</v>
       </c>
       <c r="C16">
-        <f t="shared" si="1"/>
-        <v>1666</v>
+        <v>326667</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="B17" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>F0003</v>
       </c>
       <c r="C17">
-        <f t="shared" si="1"/>
-        <v>1667</v>
+        <v>326667</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="B18" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>F0004</v>
       </c>
       <c r="C18">
-        <f t="shared" si="1"/>
-        <v>1667</v>
+        <v>6666</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="B19" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>F0005</v>
       </c>
       <c r="C19">
-        <f t="shared" si="1"/>
-        <v>1667</v>
+        <v>6666</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="B20" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>F0006</v>
       </c>
       <c r="C20">
-        <f t="shared" si="1"/>
-        <v>1667</v>
+        <v>6666</v>
       </c>
       <c r="D20">
-        <f>SUM(C9:C20)</f>
-        <v>20000</v>
+        <f>SUM(C15:C20)</f>
+        <v>1000000</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -5938,82 +6851,80 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>F0001</v>
       </c>
       <c r="C21">
-        <f t="shared" si="1"/>
-        <v>1666</v>
+        <v>321668</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
-        <f t="shared" ref="A22" si="5">A21</f>
+        <f t="shared" ref="A22" si="4">A21</f>
         <v>4</v>
       </c>
       <c r="B22" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>F0002</v>
       </c>
       <c r="C22">
-        <f t="shared" si="1"/>
-        <v>1666</v>
+        <v>321667</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="B23" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>F0003</v>
       </c>
       <c r="C23">
-        <f t="shared" si="1"/>
-        <v>1667</v>
+        <v>321667</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="B24" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>F0004</v>
       </c>
       <c r="C24">
-        <f t="shared" si="1"/>
-        <v>1667</v>
+        <v>11666</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="B25" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>F0005</v>
       </c>
       <c r="C25">
-        <f t="shared" si="1"/>
-        <v>1667</v>
+        <v>11666</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="B26" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>F0006</v>
       </c>
       <c r="C26">
-        <f t="shared" si="1"/>
-        <v>1667</v>
+        <v>11666</v>
+      </c>
+      <c r="D26">
+        <f>SUM(C21:C26)</f>
+        <v>1000000</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -6021,82 +6932,495 @@
         <v>5</v>
       </c>
       <c r="B27" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>F0001</v>
       </c>
       <c r="C27">
-        <f t="shared" si="1"/>
-        <v>1666</v>
+        <v>316668</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
-        <f t="shared" ref="A28" si="6">A27</f>
+        <f t="shared" ref="A28" si="5">A27</f>
         <v>5</v>
       </c>
       <c r="B28" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>F0002</v>
       </c>
       <c r="C28">
-        <f t="shared" si="1"/>
-        <v>1666</v>
+        <v>316667</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="B29" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>F0003</v>
       </c>
       <c r="C29">
-        <f t="shared" si="1"/>
-        <v>1667</v>
+        <v>316667</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="B30" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>F0004</v>
       </c>
       <c r="C30">
-        <f t="shared" si="1"/>
-        <v>1667</v>
+        <v>16666</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="B31" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>F0005</v>
       </c>
       <c r="C31">
-        <f t="shared" si="1"/>
-        <v>1667</v>
+        <v>16666</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="B32" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>F0006</v>
       </c>
       <c r="C32">
-        <f t="shared" si="1"/>
-        <v>1667</v>
+        <v>16666</v>
+      </c>
+      <c r="D32">
+        <f>SUM(C27:C32)</f>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>6</v>
+      </c>
+      <c r="B33" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>F0001</v>
+      </c>
+      <c r="C33">
+        <v>308334</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <f t="shared" ref="A34:A62" si="6">A33</f>
+        <v>6</v>
+      </c>
+      <c r="B34" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>F0002</v>
+      </c>
+      <c r="C34">
+        <v>308333</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="B35" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>F0003</v>
+      </c>
+      <c r="C35">
+        <v>308333</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="B36" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>F0004</v>
+      </c>
+      <c r="C36">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="B37" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>F0005</v>
+      </c>
+      <c r="C37">
+        <f t="shared" ref="C37:C38" si="7">C36</f>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="B38" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>F0006</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="7"/>
+        <v>25000</v>
+      </c>
+      <c r="D38">
+        <f t="shared" ref="D38" si="8">SUM(C33:C38)</f>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>7</v>
+      </c>
+      <c r="B39" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>F0001</v>
+      </c>
+      <c r="C39">
+        <v>300001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="B40" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>F0002</v>
+      </c>
+      <c r="C40">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="B41" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>F0003</v>
+      </c>
+      <c r="C41">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="B42" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>F0004</v>
+      </c>
+      <c r="C42">
+        <v>33333</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="B43" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>F0005</v>
+      </c>
+      <c r="C43">
+        <f t="shared" ref="C43:C44" si="9">C42</f>
+        <v>33333</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="B44" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>F0006</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="9"/>
+        <v>33333</v>
+      </c>
+      <c r="D44">
+        <f t="shared" ref="D44" si="10">SUM(C39:C44)</f>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>8</v>
+      </c>
+      <c r="B45" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>F0001</v>
+      </c>
+      <c r="C45">
+        <v>283334</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="B46" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>F0002</v>
+      </c>
+      <c r="C46">
+        <v>283333</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="B47" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>F0003</v>
+      </c>
+      <c r="C47">
+        <v>283333</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="B48" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>F0004</v>
+      </c>
+      <c r="C48">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="B49" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>F0005</v>
+      </c>
+      <c r="C49">
+        <f t="shared" ref="C49:C50" si="11">C48</f>
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="B50" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>F0006</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="11"/>
+        <v>50000</v>
+      </c>
+      <c r="D50">
+        <f t="shared" ref="D50" si="12">SUM(C45:C50)</f>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>9</v>
+      </c>
+      <c r="B51" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>F0001</v>
+      </c>
+      <c r="C51">
+        <v>266668</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="B52" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>F0002</v>
+      </c>
+      <c r="C52">
+        <v>266667</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="B53" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>F0003</v>
+      </c>
+      <c r="C53">
+        <v>266667</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="B54" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>F0004</v>
+      </c>
+      <c r="C54">
+        <v>66666</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="B55" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>F0005</v>
+      </c>
+      <c r="C55">
+        <f t="shared" ref="C55:C56" si="13">C54</f>
+        <v>66666</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="B56" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>F0006</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="13"/>
+        <v>66666</v>
+      </c>
+      <c r="D56">
+        <f t="shared" ref="D56" si="14">SUM(C51:C56)</f>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>10</v>
+      </c>
+      <c r="B57" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>F0001</v>
+      </c>
+      <c r="C57">
+        <v>233334</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="B58" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>F0002</v>
+      </c>
+      <c r="C58">
+        <v>233333</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="B59" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>F0003</v>
+      </c>
+      <c r="C59">
+        <v>233333</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="B60" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>F0004</v>
+      </c>
+      <c r="C60">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="B61" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>F0005</v>
+      </c>
+      <c r="C61">
+        <f t="shared" ref="C61:C62" si="15">C60</f>
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="B62" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>F0006</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="15"/>
+        <v>100000</v>
+      </c>
+      <c r="D62">
+        <f t="shared" ref="D62" si="16">SUM(C57:C62)</f>
+        <v>1000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[🛠️Fix] Summon Probability fix
- 동료, 스킬 소환 확률 수정
</commit_message>
<xml_diff>
--- a/IdleGame/Assets/@Resources/Texts/ExcelTable/SummonTable.xlsx
+++ b/IdleGame/Assets/@Resources/Texts/ExcelTable/SummonTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\TeamProject-IdleGame\IdleGame\Assets\@Resources\Texts\ExcelTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D0792F-D634-4BD9-A0C7-CDE69EAC7EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5ADE4F2-9CFD-4A35-806E-3047E119C61B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="91">
   <si>
     <t>Probability : Int</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -281,13 +281,43 @@
   </si>
   <si>
     <t>S0015</t>
+  </si>
+  <si>
+    <t>S0001</t>
+  </si>
+  <si>
+    <t>F0007</t>
+  </si>
+  <si>
+    <t>F0008</t>
+  </si>
+  <si>
+    <t>F0009</t>
+  </si>
+  <si>
+    <t>F0010</t>
+  </si>
+  <si>
+    <t>F0011</t>
+  </si>
+  <si>
+    <t>F0012</t>
+  </si>
+  <si>
+    <t>F0013</t>
+  </si>
+  <si>
+    <t>F0014</t>
+  </si>
+  <si>
+    <t>F0015</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -297,6 +327,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -323,11 +361,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -368,8 +407,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EB499717-A1AC-43E5-BB07-2DDEA916DCA8}" name="표1_3" displayName="표1_3" ref="A2:C122" totalsRowShown="0">
-  <autoFilter ref="A2:C122" xr:uid="{EB499717-A1AC-43E5-BB07-2DDEA916DCA8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EB499717-A1AC-43E5-BB07-2DDEA916DCA8}" name="표1_3" displayName="표1_3" ref="A2:C110" totalsRowShown="0">
+  <autoFilter ref="A2:C110" xr:uid="{EB499717-A1AC-43E5-BB07-2DDEA916DCA8}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{06FEEBCF-143F-467A-94A3-ED6516C27AF9}" name="SummonGrade : Int"/>
     <tableColumn id="2" xr3:uid="{94EF72E9-ADB9-4815-8659-1DBA16E8F4CA}" name="ItemId : String" dataDxfId="1"/>
@@ -380,8 +419,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5A4DFF02-36B8-41E7-8806-3F9C3960FF2C}" name="표1_34" displayName="표1_34" ref="A2:C62" totalsRowShown="0">
-  <autoFilter ref="A2:C62" xr:uid="{5A4DFF02-36B8-41E7-8806-3F9C3960FF2C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5A4DFF02-36B8-41E7-8806-3F9C3960FF2C}" name="표1_34" displayName="표1_34" ref="A2:C110" totalsRowShown="0">
+  <autoFilter ref="A2:C110" xr:uid="{5A4DFF02-36B8-41E7-8806-3F9C3960FF2C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{33B2D4D5-FB6D-4D4D-BFB4-929061FDF8C7}" name="SummonGrade : Int"/>
     <tableColumn id="2" xr3:uid="{ED56F630-FCAF-4415-A242-47AC6BE1C32C}" name="ItemId : String" dataDxfId="0"/>
@@ -5025,10 +5064,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E6FFAFD-B9D4-4D16-9C10-FE1E60CA3279}">
-  <dimension ref="A1:C122"/>
+  <dimension ref="A1:C123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="C110" sqref="A3:C110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5062,7 +5101,7 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>200000</v>
+        <v>266668</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -5074,19 +5113,19 @@
         <v>11</v>
       </c>
       <c r="C4">
-        <v>200000</v>
+        <v>266667</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f t="shared" ref="A5:A17" si="0">A4</f>
+        <f t="shared" ref="A5:A18" si="0">A4</f>
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C5">
-        <v>200000</v>
+        <v>266667</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -5098,7 +5137,7 @@
         <v>13</v>
       </c>
       <c r="C6">
-        <v>200000</v>
+        <v>66666</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -5110,163 +5149,156 @@
         <v>14</v>
       </c>
       <c r="C7">
-        <v>200000</v>
+        <v>66666</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C8">
-        <v>198000</v>
+        <v>66666</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
-        <f>A8</f>
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>81</v>
       </c>
       <c r="C9">
-        <v>198000</v>
+        <v>258334</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
-        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10">
-        <v>198000</v>
+        <v>258333</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
-        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11">
-        <v>198000</v>
+        <v>258333</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
-        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12">
-        <v>198000</v>
+        <v>75000</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
-        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13">
-        <v>2000</v>
+        <v>75000</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
-        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14">
-        <v>2000</v>
+        <v>75000</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>81</v>
       </c>
       <c r="C15">
-        <v>2000</v>
+        <v>246668</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>A15</f>
+        <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C16">
-        <v>2000</v>
+        <v>246667</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f t="shared" ref="A17:A23" si="1">A16</f>
+        <v>3</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>75</v>
+        <v>12</v>
       </c>
       <c r="C17">
-        <v>2000</v>
+        <v>246667</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C18">
-        <v>196000</v>
+        <v>83333</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
-        <f>A18</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C19">
-        <f>C18</f>
-        <v>196000</v>
+        <v>83333</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
-        <f t="shared" ref="A20:A27" si="1">A19</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C20">
-        <f t="shared" ref="C20:C22" si="2">C19</f>
-        <v>196000</v>
+        <v>83333</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -5275,11 +5307,10 @@
         <v>3</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C21">
-        <f t="shared" si="2"/>
-        <v>196000</v>
+        <v>3333</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -5288,11 +5319,10 @@
         <v>3</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C22">
-        <f t="shared" si="2"/>
-        <v>196000</v>
+        <v>3333</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -5301,1272 +5331,1087 @@
         <v>3</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C23">
-        <v>4000</v>
+        <v>3333</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="C24">
-        <f>C23</f>
-        <v>4000</v>
+        <v>243335</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <f>A24</f>
+        <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C25">
-        <f t="shared" ref="C25:C27" si="3">C24</f>
-        <v>4000</v>
+        <v>243334</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <f t="shared" ref="A26:A32" si="2">A25</f>
+        <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C26">
-        <f t="shared" si="3"/>
-        <v>4000</v>
+        <v>243334</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>75</v>
+        <v>13</v>
       </c>
       <c r="C27">
-        <f t="shared" si="3"/>
-        <v>4000</v>
+        <v>83333</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C28">
-        <v>193000</v>
+        <v>83333</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
-        <f>A28</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C29">
-        <f>C28</f>
-        <v>193000</v>
+        <v>83333</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
-        <f t="shared" ref="A30:A37" si="4">A29</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C30">
-        <f t="shared" ref="C30:C32" si="5">C29</f>
-        <v>193000</v>
+        <v>6666</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C31">
-        <f t="shared" si="5"/>
-        <v>193000</v>
+        <v>6666</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C32">
-        <f t="shared" si="5"/>
-        <v>193000</v>
+        <v>6666</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
-        <f t="shared" si="4"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="C33">
-        <v>7000</v>
+        <v>220001</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
-        <f t="shared" si="4"/>
-        <v>4</v>
+        <f>A33</f>
+        <v>5</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C34">
-        <f>C33</f>
-        <v>7000</v>
+        <v>220000</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
-        <f t="shared" si="4"/>
-        <v>4</v>
+        <f t="shared" ref="A35:A41" si="3">A34</f>
+        <v>5</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C35">
-        <f t="shared" ref="C35:C37" si="6">C34</f>
-        <v>7000</v>
+        <v>220000</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
-        <f t="shared" si="4"/>
-        <v>4</v>
+        <f t="shared" si="3"/>
+        <v>5</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C36">
-        <f t="shared" si="6"/>
-        <v>7000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
-        <f t="shared" si="4"/>
-        <v>4</v>
+        <f t="shared" si="3"/>
+        <v>5</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
       <c r="C37">
-        <f t="shared" si="6"/>
-        <v>7000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C38">
-        <v>190000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
-        <f>A38</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C39">
-        <f>C38</f>
-        <v>190000</v>
+        <v>13333</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
-        <f t="shared" ref="A40:A62" si="7">A39</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C40">
-        <f t="shared" ref="C40:C42" si="8">C39</f>
-        <v>190000</v>
+        <v>13333</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C41">
-        <f t="shared" si="8"/>
-        <v>190000</v>
+        <v>13333</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
-        <f t="shared" si="7"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="C42">
-        <f t="shared" si="8"/>
-        <v>190000</v>
+        <v>210001</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43">
-        <f t="shared" si="7"/>
-        <v>5</v>
+        <f>A42</f>
+        <v>6</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C43">
-        <v>10000</v>
+        <v>210000</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44">
-        <f t="shared" si="7"/>
-        <v>5</v>
+        <f t="shared" ref="A44:A50" si="4">A43</f>
+        <v>6</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C44">
-        <f>C43</f>
-        <v>10000</v>
+        <v>210000</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
-        <f t="shared" si="7"/>
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>6</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C45">
-        <f t="shared" ref="C45:C47" si="9">C44</f>
-        <v>10000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
-        <f t="shared" si="7"/>
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>6</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C46">
-        <f t="shared" si="9"/>
-        <v>10000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47">
-        <f t="shared" si="7"/>
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>6</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>75</v>
+        <v>15</v>
       </c>
       <c r="C47">
-        <f t="shared" si="9"/>
-        <v>10000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C48">
-        <v>184900</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49">
-        <f>A48</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C49">
-        <f>C48</f>
-        <v>184900</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C50">
-        <f t="shared" ref="C50:C52" si="10">C49</f>
-        <v>184900</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="A51:A53" si="5">A50</f>
         <v>6</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="C51">
-        <f t="shared" si="10"/>
-        <v>184900</v>
+        <v>3333</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="C52">
-        <f t="shared" si="10"/>
-        <v>184900</v>
+        <v>3333</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>15</v>
+        <v>77</v>
       </c>
       <c r="C53">
-        <v>15000</v>
+        <v>3333</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54">
-        <f t="shared" si="7"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="C54">
-        <f>C53</f>
-        <v>15000</v>
+        <v>183336</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55">
-        <f t="shared" si="7"/>
-        <v>6</v>
+        <f>A54</f>
+        <v>7</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C55">
-        <f t="shared" ref="C55:C57" si="11">C54</f>
-        <v>15000</v>
+        <v>183335</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56">
-        <f t="shared" si="7"/>
-        <v>6</v>
+        <f t="shared" ref="A56:A65" si="6">A55</f>
+        <v>7</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C56">
-        <f t="shared" si="11"/>
-        <v>15000</v>
+        <v>183335</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57">
-        <f t="shared" si="7"/>
-        <v>6</v>
+        <f t="shared" si="6"/>
+        <v>7</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>75</v>
+        <v>13</v>
       </c>
       <c r="C57">
-        <f t="shared" si="11"/>
-        <v>15000</v>
+        <v>116666</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58">
-        <f t="shared" si="7"/>
-        <v>6</v>
+        <f t="shared" si="6"/>
+        <v>7</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>76</v>
+        <v>14</v>
       </c>
       <c r="C58">
-        <v>100</v>
+        <v>116666</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59">
-        <f t="shared" si="7"/>
-        <v>6</v>
+        <f t="shared" si="6"/>
+        <v>7</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="C59">
-        <f>C58</f>
-        <v>100</v>
+        <v>116666</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60">
-        <f t="shared" si="7"/>
-        <v>6</v>
+        <f t="shared" si="6"/>
+        <v>7</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>78</v>
+        <v>16</v>
       </c>
       <c r="C60">
-        <f t="shared" ref="C60:C62" si="12">C59</f>
-        <v>100</v>
+        <v>26666</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61">
-        <f t="shared" si="7"/>
-        <v>6</v>
+        <f t="shared" si="6"/>
+        <v>7</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>79</v>
+        <v>17</v>
       </c>
       <c r="C61">
-        <f t="shared" si="12"/>
-        <v>100</v>
+        <v>26666</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62">
-        <f t="shared" si="7"/>
-        <v>6</v>
+        <f t="shared" si="6"/>
+        <v>7</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>80</v>
+        <v>18</v>
       </c>
       <c r="C62">
-        <f t="shared" si="12"/>
-        <v>100</v>
+        <v>26666</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63">
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>10</v>
+        <v>75</v>
       </c>
       <c r="C63">
-        <v>179800</v>
+        <v>6666</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64">
-        <f>A63</f>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>11</v>
+        <v>76</v>
       </c>
       <c r="C64">
-        <f>C63</f>
-        <v>179800</v>
+        <v>6666</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65">
-        <f t="shared" ref="A65:A77" si="13">A64</f>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="C65">
-        <f t="shared" ref="C65:C67" si="14">C64</f>
-        <v>179800</v>
+        <v>6666</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66">
-        <f t="shared" si="13"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="C66">
-        <f t="shared" si="14"/>
-        <v>179800</v>
+        <v>169669</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67">
-        <f t="shared" si="13"/>
-        <v>7</v>
+        <f>A66</f>
+        <v>8</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C67">
-        <f t="shared" si="14"/>
-        <v>179800</v>
+        <v>169668</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68">
-        <f t="shared" si="13"/>
-        <v>7</v>
+        <f t="shared" ref="A68:A77" si="7">A67</f>
+        <v>8</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C68">
-        <v>20000</v>
+        <v>169668</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69">
-        <f t="shared" si="13"/>
-        <v>7</v>
+        <f t="shared" si="7"/>
+        <v>8</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C69">
-        <f>C68</f>
-        <v>20000</v>
+        <v>116666</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70">
-        <f t="shared" si="13"/>
-        <v>7</v>
+        <f t="shared" si="7"/>
+        <v>8</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C70">
-        <f t="shared" ref="C70:C72" si="15">C69</f>
-        <v>20000</v>
+        <v>116666</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71">
-        <f t="shared" si="13"/>
-        <v>7</v>
+        <f t="shared" si="7"/>
+        <v>8</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C71">
-        <f t="shared" si="15"/>
-        <v>20000</v>
+        <v>116666</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72">
-        <f t="shared" si="13"/>
-        <v>7</v>
+        <f t="shared" si="7"/>
+        <v>8</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>75</v>
+        <v>16</v>
       </c>
       <c r="C72">
-        <f t="shared" si="15"/>
-        <v>20000</v>
+        <v>33333</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73">
-        <f t="shared" si="13"/>
-        <v>7</v>
+        <f t="shared" si="7"/>
+        <v>8</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="C73">
-        <v>200</v>
+        <v>33333</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74">
-        <f t="shared" si="13"/>
-        <v>7</v>
+        <f t="shared" si="7"/>
+        <v>8</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>77</v>
+        <v>18</v>
       </c>
       <c r="C74">
-        <f>C73</f>
-        <v>200</v>
+        <v>33333</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75">
-        <f t="shared" si="13"/>
-        <v>7</v>
+        <f t="shared" si="7"/>
+        <v>8</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C75">
-        <f t="shared" ref="C75:C77" si="16">C74</f>
-        <v>200</v>
+        <v>13333</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76">
-        <f t="shared" si="13"/>
-        <v>7</v>
+        <f t="shared" si="7"/>
+        <v>8</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C76">
-        <f t="shared" si="16"/>
-        <v>200</v>
+        <v>13333</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77">
-        <f t="shared" si="13"/>
-        <v>7</v>
+        <f t="shared" si="7"/>
+        <v>8</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C77">
-        <f t="shared" si="16"/>
-        <v>200</v>
+        <v>13333</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78">
+        <f t="shared" ref="A78:A80" si="8">A77</f>
         <v>8</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>10</v>
+        <v>78</v>
       </c>
       <c r="C78">
-        <v>169200</v>
+        <v>333</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79">
-        <f>A78</f>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>11</v>
+        <v>79</v>
       </c>
       <c r="C79">
-        <f>C78</f>
-        <v>169200</v>
+        <v>333</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80">
-        <f t="shared" ref="A80:A92" si="17">A79</f>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="C80">
-        <f t="shared" ref="C80:C82" si="18">C79</f>
-        <v>169200</v>
+        <v>333</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81">
-        <f t="shared" si="17"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="C81">
-        <f t="shared" si="18"/>
-        <v>169200</v>
+        <v>137002</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82">
-        <f t="shared" si="17"/>
-        <v>8</v>
+        <f>A81</f>
+        <v>9</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C82">
-        <f t="shared" si="18"/>
-        <v>169200</v>
+        <v>137001</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83">
-        <f t="shared" si="17"/>
-        <v>8</v>
+        <f t="shared" ref="A83:A95" si="9">A82</f>
+        <v>9</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C83">
-        <v>30000</v>
+        <v>137001</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84">
-        <f t="shared" si="17"/>
-        <v>8</v>
+        <f t="shared" si="9"/>
+        <v>9</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C84">
-        <f>C83</f>
-        <v>30000</v>
+        <v>133333</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85">
-        <f t="shared" si="17"/>
-        <v>8</v>
+        <f t="shared" si="9"/>
+        <v>9</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C85">
-        <f t="shared" ref="C85:C87" si="19">C84</f>
-        <v>30000</v>
+        <v>133333</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86">
-        <f t="shared" si="17"/>
-        <v>8</v>
+        <f t="shared" si="9"/>
+        <v>9</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C86">
-        <f t="shared" si="19"/>
-        <v>30000</v>
+        <v>133333</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87">
-        <f t="shared" si="17"/>
-        <v>8</v>
+        <f t="shared" si="9"/>
+        <v>9</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>75</v>
+        <v>16</v>
       </c>
       <c r="C87">
-        <f t="shared" si="19"/>
-        <v>30000</v>
+        <v>41666</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88">
-        <f t="shared" si="17"/>
-        <v>8</v>
+        <f t="shared" si="9"/>
+        <v>9</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="C88">
-        <v>800</v>
+        <v>41666</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89">
-        <f t="shared" si="17"/>
-        <v>8</v>
+        <f t="shared" si="9"/>
+        <v>9</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>77</v>
+        <v>18</v>
       </c>
       <c r="C89">
-        <f>C88</f>
-        <v>800</v>
+        <v>41666</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90">
-        <f t="shared" si="17"/>
-        <v>8</v>
+        <f t="shared" si="9"/>
+        <v>9</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C90">
-        <f t="shared" ref="C90:C92" si="20">C89</f>
-        <v>800</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91">
-        <f t="shared" si="17"/>
-        <v>8</v>
+        <f t="shared" si="9"/>
+        <v>9</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C91">
-        <f t="shared" si="20"/>
-        <v>800</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92">
-        <f t="shared" si="17"/>
-        <v>8</v>
+        <f t="shared" si="9"/>
+        <v>9</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C92">
-        <f t="shared" si="20"/>
-        <v>800</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93">
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>10</v>
+        <v>78</v>
       </c>
       <c r="C93">
-        <v>158600</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94">
-        <f>A93</f>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>11</v>
+        <v>79</v>
       </c>
       <c r="C94">
-        <f>C93</f>
-        <v>158600</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95">
-        <f t="shared" ref="A95:A107" si="21">A94</f>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="C95">
-        <f t="shared" ref="C95:C97" si="22">C94</f>
-        <v>158600</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96">
-        <f t="shared" si="21"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C96">
-        <f t="shared" si="22"/>
-        <v>158600</v>
+        <v>81</v>
+      </c>
+      <c r="C96" s="2">
+        <v>120002</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97">
-        <f t="shared" si="21"/>
-        <v>9</v>
+        <f>A96</f>
+        <v>10</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C97">
-        <f t="shared" si="22"/>
-        <v>158600</v>
+        <v>11</v>
+      </c>
+      <c r="C97" s="2">
+        <v>120001</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98">
-        <f t="shared" si="21"/>
-        <v>9</v>
+        <f t="shared" ref="A98:A110" si="10">A97</f>
+        <v>10</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C98">
-        <v>40000</v>
+        <v>12</v>
+      </c>
+      <c r="C98" s="2">
+        <v>120001</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99">
-        <f t="shared" si="21"/>
-        <v>9</v>
+        <f t="shared" si="10"/>
+        <v>10</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C99">
-        <f>C98</f>
-        <v>40000</v>
+        <v>133333</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100">
-        <f t="shared" si="21"/>
-        <v>9</v>
+        <f t="shared" si="10"/>
+        <v>10</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C100">
-        <f t="shared" ref="C100:C102" si="23">C99</f>
-        <v>40000</v>
+        <v>133333</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101">
-        <f t="shared" si="21"/>
-        <v>9</v>
+        <f t="shared" si="10"/>
+        <v>10</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C101">
-        <f t="shared" si="23"/>
-        <v>40000</v>
+        <v>133333</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102">
-        <f t="shared" si="21"/>
-        <v>9</v>
+        <f t="shared" si="10"/>
+        <v>10</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>75</v>
+        <v>16</v>
       </c>
       <c r="C102">
-        <f t="shared" si="23"/>
-        <v>40000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103">
-        <f t="shared" si="21"/>
-        <v>9</v>
+        <f t="shared" si="10"/>
+        <v>10</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="C103">
-        <v>1400</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104">
-        <f t="shared" si="21"/>
-        <v>9</v>
+        <f t="shared" si="10"/>
+        <v>10</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>77</v>
+        <v>18</v>
       </c>
       <c r="C104">
-        <f>C103</f>
-        <v>1400</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105">
-        <f t="shared" si="21"/>
-        <v>9</v>
+        <f t="shared" si="10"/>
+        <v>10</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C105">
-        <f t="shared" ref="C105:C107" si="24">C104</f>
-        <v>1400</v>
+        <v>26666</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106">
-        <f t="shared" si="21"/>
-        <v>9</v>
+        <f t="shared" si="10"/>
+        <v>10</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C106">
-        <f t="shared" si="24"/>
-        <v>1400</v>
+        <v>26666</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107">
-        <f t="shared" si="21"/>
-        <v>9</v>
+        <f t="shared" si="10"/>
+        <v>10</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C107">
-        <f t="shared" si="24"/>
-        <v>1400</v>
+        <v>26666</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108">
+        <f t="shared" si="10"/>
         <v>10</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>10</v>
+        <v>78</v>
       </c>
       <c r="C108">
-        <v>138000</v>
+        <v>3333</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109">
-        <f>A108</f>
+        <f t="shared" si="10"/>
         <v>10</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>11</v>
+        <v>79</v>
       </c>
       <c r="C109">
-        <f>C108</f>
-        <v>138000</v>
+        <v>3333</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110">
-        <f t="shared" ref="A110:A122" si="25">A109</f>
+        <f t="shared" si="10"/>
         <v>10</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="C110">
-        <f t="shared" ref="C110:C112" si="26">C109</f>
-        <v>138000</v>
+        <v>3333</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A111">
-        <f t="shared" si="25"/>
-        <v>10</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C111">
-        <f t="shared" si="26"/>
-        <v>138000</v>
-      </c>
+      <c r="B111" s="1"/>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A112">
-        <f t="shared" si="25"/>
-        <v>10</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C112">
-        <f t="shared" si="26"/>
-        <v>138000</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A113">
-        <f t="shared" si="25"/>
-        <v>10</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C113">
-        <v>60000</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A114">
-        <f t="shared" si="25"/>
-        <v>10</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C114">
-        <f>C113</f>
-        <v>60000</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A115">
-        <f t="shared" si="25"/>
-        <v>10</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C115">
-        <f t="shared" ref="C115:C117" si="27">C114</f>
-        <v>60000</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A116">
-        <f t="shared" si="25"/>
-        <v>10</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C116">
-        <f t="shared" si="27"/>
-        <v>60000</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A117">
-        <f t="shared" si="25"/>
-        <v>10</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C117">
-        <f t="shared" si="27"/>
-        <v>60000</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A118">
-        <f t="shared" si="25"/>
-        <v>10</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C118">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A119">
-        <f t="shared" si="25"/>
-        <v>10</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C119">
-        <f>C118</f>
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A120">
-        <f t="shared" si="25"/>
-        <v>10</v>
-      </c>
-      <c r="B120" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C120">
-        <f t="shared" ref="C120:C122" si="28">C119</f>
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A121">
-        <f t="shared" si="25"/>
-        <v>10</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C121">
-        <f t="shared" si="28"/>
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A122">
-        <f t="shared" si="25"/>
-        <v>10</v>
-      </c>
-      <c r="B122" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C122">
-        <f t="shared" si="28"/>
-        <v>2000</v>
-      </c>
+      <c r="B112" s="1"/>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B113" s="1"/>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B114" s="1"/>
+    </row>
+    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B115" s="1"/>
+    </row>
+    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B116" s="1"/>
+    </row>
+    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B117" s="1"/>
+    </row>
+    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B118" s="1"/>
+    </row>
+    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B119" s="1"/>
+    </row>
+    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B120" s="1"/>
+    </row>
+    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B121" s="1"/>
+    </row>
+    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B122" s="1"/>
+    </row>
+    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B123" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -6580,10 +6425,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF1FBEA-E97D-46D7-B77D-7F9DD3257CDE}">
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:D110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6617,7 +6462,7 @@
         <v>21</v>
       </c>
       <c r="C3">
-        <v>333334</v>
+        <v>266668</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -6629,7 +6474,7 @@
         <v>22</v>
       </c>
       <c r="C4">
-        <v>333333</v>
+        <v>266667</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -6641,7 +6486,7 @@
         <v>23</v>
       </c>
       <c r="C5">
-        <v>333333</v>
+        <v>266667</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -6653,7 +6498,7 @@
         <v>24</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>66666</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -6665,7 +6510,7 @@
         <v>25</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>66666</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -6677,7 +6522,7 @@
         <v>26</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>66666</v>
       </c>
       <c r="D8">
         <f>SUM(C3:C8)</f>
@@ -6688,77 +6533,66 @@
       <c r="A9">
         <v>2</v>
       </c>
-      <c r="B9" s="1" t="str">
-        <f>B3</f>
-        <v>F0001</v>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C9">
-        <v>330001</v>
+        <v>258334</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
-        <f>A9</f>
         <v>2</v>
       </c>
-      <c r="B10" s="1" t="str">
-        <f>B4</f>
-        <v>F0002</v>
+      <c r="B10" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C10">
-        <v>330000</v>
+        <v>258333</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
-        <f t="shared" ref="A11:A14" si="1">A10</f>
         <v>2</v>
       </c>
-      <c r="B11" s="1" t="str">
-        <f>B5</f>
-        <v>F0003</v>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="C11">
-        <v>330000</v>
+        <v>258333</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="B12" s="1" t="str">
-        <f>B6</f>
-        <v>F0004</v>
+      <c r="B12" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C12">
-        <v>3333</v>
+        <v>75000</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="B13" s="1" t="str">
-        <f>B7</f>
-        <v>F0005</v>
+      <c r="B13" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="C13">
-        <v>3333</v>
+        <v>75000</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="B14" s="1" t="str">
-        <f>B8</f>
-        <v>F0006</v>
+      <c r="B14" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C14">
-        <v>3333</v>
+        <v>75000</v>
       </c>
       <c r="D14">
         <f>SUM(C9:C14)</f>
@@ -6769,658 +6603,1176 @@
       <c r="A15">
         <v>3</v>
       </c>
-      <c r="B15" s="1" t="str">
-        <f t="shared" ref="B15:B62" si="2">B9</f>
-        <v>F0001</v>
+      <c r="B15" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C15">
-        <v>326668</v>
+        <v>246668</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
-        <f t="shared" ref="A16:A32" si="3">A15</f>
+        <f>A15</f>
         <v>3</v>
       </c>
-      <c r="B16" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0002</v>
+      <c r="B16" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C16">
-        <v>326667</v>
+        <v>246667</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="A17:A23" si="1">A16</f>
         <v>3</v>
       </c>
-      <c r="B17" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0003</v>
+      <c r="B17" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="C17">
-        <v>326667</v>
+        <v>246667</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B18" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0004</v>
+      <c r="B18" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C18">
-        <v>6666</v>
+        <v>83333</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B19" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0005</v>
+      <c r="B19" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="C19">
-        <v>6666</v>
+        <v>83333</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B20" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0006</v>
+      <c r="B20" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C20">
-        <v>6666</v>
+        <v>83333</v>
       </c>
       <c r="D20">
         <f>SUM(C15:C20)</f>
-        <v>1000000</v>
+        <v>990001</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>4</v>
-      </c>
-      <c r="B21" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0001</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="C21">
-        <v>321668</v>
+        <v>3333</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
-        <f t="shared" ref="A22" si="4">A21</f>
-        <v>4</v>
-      </c>
-      <c r="B22" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0002</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="C22">
-        <v>321667</v>
+        <v>3333</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="B23" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0003</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="C23">
-        <v>321667</v>
+        <v>3333</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
-        <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="B24" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0004</v>
+      <c r="B24" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C24">
-        <v>11666</v>
+        <v>243335</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
-        <f t="shared" si="3"/>
+        <f>A24</f>
         <v>4</v>
       </c>
-      <c r="B25" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0005</v>
+      <c r="B25" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C25">
-        <v>11666</v>
+        <v>243334</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="A26:A32" si="2">A25</f>
         <v>4</v>
       </c>
-      <c r="B26" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0006</v>
+      <c r="B26" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="C26">
-        <v>11666</v>
+        <v>243334</v>
       </c>
       <c r="D26">
         <f>SUM(C21:C26)</f>
-        <v>1000000</v>
+        <v>740002</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>5</v>
-      </c>
-      <c r="B27" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>F0001</v>
+        <v>4</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C27">
-        <v>316668</v>
+        <v>83333</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
-        <f t="shared" ref="A28" si="5">A27</f>
-        <v>5</v>
-      </c>
-      <c r="B28" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>F0002</v>
+        <v>4</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="C28">
-        <v>316667</v>
+        <v>83333</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29">
+        <v>83333</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30">
+        <v>6666</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31">
+        <v>6666</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32">
+        <v>6666</v>
+      </c>
+      <c r="D32">
+        <f>SUM(C27:C32)</f>
+        <v>269997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>5</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33">
+        <v>220001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <f>A33</f>
+        <v>5</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34">
+        <v>220000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <f t="shared" ref="A35:A41" si="3">A34</f>
+        <v>5</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35">
+        <v>220000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="B29" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0003</v>
-      </c>
-      <c r="C29">
-        <v>316667</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30">
+      <c r="B36" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="B30" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0004</v>
-      </c>
-      <c r="C30">
-        <v>16666</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31">
+      <c r="B37" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="B31" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0005</v>
-      </c>
-      <c r="C31">
-        <v>16666</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32">
+      <c r="B38" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C38">
+        <v>100000</v>
+      </c>
+      <c r="D38">
+        <f t="shared" ref="D38" si="4">SUM(C33:C38)</f>
+        <v>960001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="B32" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0006</v>
-      </c>
-      <c r="C32">
-        <v>16666</v>
-      </c>
-      <c r="D32">
-        <f>SUM(C27:C32)</f>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <v>6</v>
-      </c>
-      <c r="B33" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0001</v>
-      </c>
-      <c r="C33">
-        <v>308334</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <f t="shared" ref="A34:A62" si="6">A33</f>
-        <v>6</v>
-      </c>
-      <c r="B34" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0002</v>
-      </c>
-      <c r="C34">
-        <v>308333</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35">
-        <f t="shared" si="6"/>
-        <v>6</v>
-      </c>
-      <c r="B35" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0003</v>
-      </c>
-      <c r="C35">
-        <v>308333</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36">
-        <f t="shared" si="6"/>
-        <v>6</v>
-      </c>
-      <c r="B36" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0004</v>
-      </c>
-      <c r="C36">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <f t="shared" si="6"/>
-        <v>6</v>
-      </c>
-      <c r="B37" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0005</v>
-      </c>
-      <c r="C37">
-        <f t="shared" ref="C37:C38" si="7">C36</f>
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38">
-        <f t="shared" si="6"/>
-        <v>6</v>
-      </c>
-      <c r="B38" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0006</v>
-      </c>
-      <c r="C38">
-        <f t="shared" si="7"/>
-        <v>25000</v>
-      </c>
-      <c r="D38">
-        <f t="shared" ref="D38" si="8">SUM(C33:C38)</f>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <v>7</v>
-      </c>
-      <c r="B39" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0001</v>
+      <c r="B39" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="C39">
-        <v>300001</v>
+        <v>13333</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
-        <f t="shared" si="6"/>
-        <v>7</v>
-      </c>
-      <c r="B40" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0002</v>
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="C40">
-        <v>300000</v>
+        <v>13333</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
-        <f t="shared" si="6"/>
-        <v>7</v>
-      </c>
-      <c r="B41" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0003</v>
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="C41">
-        <v>300000</v>
+        <v>13333</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
-        <f t="shared" si="6"/>
-        <v>7</v>
-      </c>
-      <c r="B42" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0004</v>
+        <v>6</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C42">
-        <v>33333</v>
+        <v>210001</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
-        <f t="shared" si="6"/>
-        <v>7</v>
-      </c>
-      <c r="B43" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0005</v>
+        <f>A42</f>
+        <v>6</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C43">
-        <f t="shared" ref="C43:C44" si="9">C42</f>
-        <v>33333</v>
+        <v>210000</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
-        <f t="shared" si="6"/>
-        <v>7</v>
-      </c>
-      <c r="B44" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0006</v>
+        <f t="shared" ref="A44:A53" si="5">A43</f>
+        <v>6</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="C44">
-        <f t="shared" si="9"/>
-        <v>33333</v>
+        <v>210000</v>
       </c>
       <c r="D44">
-        <f t="shared" ref="D44" si="10">SUM(C39:C44)</f>
-        <v>1000000</v>
+        <f t="shared" ref="D44" si="6">SUM(C39:C44)</f>
+        <v>670000</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>8</v>
-      </c>
-      <c r="B45" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0001</v>
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C45">
-        <v>283334</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
-        <f t="shared" si="6"/>
-        <v>8</v>
-      </c>
-      <c r="B46" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0002</v>
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="C46">
-        <v>283333</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
-        <f t="shared" si="6"/>
-        <v>8</v>
-      </c>
-      <c r="B47" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0003</v>
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C47">
-        <v>283333</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
-        <f t="shared" si="6"/>
-        <v>8</v>
-      </c>
-      <c r="B48" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0004</v>
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="C48">
-        <v>50000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
-        <f t="shared" si="6"/>
-        <v>8</v>
-      </c>
-      <c r="B49" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0005</v>
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="C49">
-        <f t="shared" ref="C49:C50" si="11">C48</f>
-        <v>50000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
-        <f t="shared" si="6"/>
-        <v>8</v>
-      </c>
-      <c r="B50" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0006</v>
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="C50">
-        <f t="shared" si="11"/>
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="D50">
-        <f t="shared" ref="D50" si="12">SUM(C45:C50)</f>
-        <v>1000000</v>
+        <f t="shared" ref="D50" si="7">SUM(C45:C50)</f>
+        <v>360000</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>9</v>
-      </c>
-      <c r="B51" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0001</v>
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="C51">
-        <v>266668</v>
+        <v>3333</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
-        <f t="shared" si="6"/>
-        <v>9</v>
-      </c>
-      <c r="B52" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0002</v>
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="C52">
-        <v>266667</v>
+        <v>3333</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
-        <f t="shared" si="6"/>
-        <v>9</v>
-      </c>
-      <c r="B53" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0003</v>
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="C53">
-        <v>266667</v>
+        <v>3333</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
-        <f t="shared" si="6"/>
-        <v>9</v>
-      </c>
-      <c r="B54" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0004</v>
+        <v>7</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C54">
-        <v>66666</v>
+        <v>183336</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
-        <f t="shared" si="6"/>
-        <v>9</v>
-      </c>
-      <c r="B55" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0005</v>
+        <f>A54</f>
+        <v>7</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C55">
-        <f t="shared" ref="C55:C56" si="13">C54</f>
-        <v>66666</v>
+        <v>183335</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
-        <f t="shared" si="6"/>
-        <v>9</v>
-      </c>
-      <c r="B56" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0006</v>
+        <f t="shared" ref="A56:A65" si="8">A55</f>
+        <v>7</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="C56">
-        <f t="shared" si="13"/>
-        <v>66666</v>
+        <v>183335</v>
       </c>
       <c r="D56">
-        <f t="shared" ref="D56" si="14">SUM(C51:C56)</f>
-        <v>1000000</v>
+        <f t="shared" ref="D56" si="9">SUM(C51:C56)</f>
+        <v>560005</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>10</v>
-      </c>
-      <c r="B57" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0001</v>
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C57">
-        <v>233334</v>
+        <v>116666</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
-        <f t="shared" si="6"/>
-        <v>10</v>
-      </c>
-      <c r="B58" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0002</v>
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="C58">
-        <v>233333</v>
+        <v>116666</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59">
-        <f t="shared" si="6"/>
-        <v>10</v>
-      </c>
-      <c r="B59" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0003</v>
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C59">
-        <v>233333</v>
+        <v>116666</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60">
-        <f t="shared" si="6"/>
-        <v>10</v>
-      </c>
-      <c r="B60" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0004</v>
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="C60">
-        <v>100000</v>
+        <v>26666</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61">
-        <f t="shared" si="6"/>
-        <v>10</v>
-      </c>
-      <c r="B61" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0005</v>
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="C61">
-        <f t="shared" ref="C61:C62" si="15">C60</f>
-        <v>100000</v>
+        <v>26666</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62">
-        <f t="shared" si="6"/>
-        <v>10</v>
-      </c>
-      <c r="B62" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>F0006</v>
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="C62">
-        <f t="shared" si="15"/>
-        <v>100000</v>
+        <v>26666</v>
       </c>
       <c r="D62">
-        <f t="shared" ref="D62" si="16">SUM(C57:C62)</f>
-        <v>1000000</v>
+        <f t="shared" ref="D62" si="10">SUM(C57:C62)</f>
+        <v>429996</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C63">
+        <v>6666</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C64">
+        <v>6666</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C65">
+        <v>6666</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>8</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C66">
+        <v>169669</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <f>A66</f>
+        <v>8</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C67">
+        <v>169668</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <f t="shared" ref="A68:A80" si="11">A67</f>
+        <v>8</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C68">
+        <v>169668</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <f t="shared" si="11"/>
+        <v>8</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C69">
+        <v>116666</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <f t="shared" si="11"/>
+        <v>8</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C70">
+        <v>116666</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <f t="shared" si="11"/>
+        <v>8</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C71">
+        <v>116666</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <f t="shared" si="11"/>
+        <v>8</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C72">
+        <v>33333</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <f t="shared" si="11"/>
+        <v>8</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C73">
+        <v>33333</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <f t="shared" si="11"/>
+        <v>8</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C74">
+        <v>33333</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <f t="shared" si="11"/>
+        <v>8</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C75">
+        <v>13333</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <f t="shared" si="11"/>
+        <v>8</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C76">
+        <v>13333</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <f t="shared" si="11"/>
+        <v>8</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C77">
+        <v>13333</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <f t="shared" si="11"/>
+        <v>8</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C78">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <f t="shared" si="11"/>
+        <v>8</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C79">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <f t="shared" si="11"/>
+        <v>8</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C80">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>9</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C81">
+        <v>137002</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <f>A81</f>
+        <v>9</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C82">
+        <v>137001</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <f t="shared" ref="A83:A95" si="12">A82</f>
+        <v>9</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C83">
+        <v>137001</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <f t="shared" si="12"/>
+        <v>9</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C84">
+        <v>133333</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <f t="shared" si="12"/>
+        <v>9</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C85">
+        <v>133333</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <f t="shared" si="12"/>
+        <v>9</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C86">
+        <v>133333</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <f t="shared" si="12"/>
+        <v>9</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C87">
+        <v>41666</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <f t="shared" si="12"/>
+        <v>9</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C88">
+        <v>41666</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <f t="shared" si="12"/>
+        <v>9</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C89">
+        <v>41666</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <f t="shared" si="12"/>
+        <v>9</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C90">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <f t="shared" si="12"/>
+        <v>9</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C91">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <f t="shared" si="12"/>
+        <v>9</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C92">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <f t="shared" si="12"/>
+        <v>9</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C93">
+        <v>1333</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <f t="shared" si="12"/>
+        <v>9</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C94">
+        <v>1333</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <f t="shared" si="12"/>
+        <v>9</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C95">
+        <v>1333</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>10</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C96" s="2">
+        <v>120002</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <f>A96</f>
+        <v>10</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C97" s="2">
+        <v>120001</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <f t="shared" ref="A98:A110" si="13">A97</f>
+        <v>10</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C98" s="2">
+        <v>120001</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <f t="shared" si="13"/>
+        <v>10</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C99">
+        <v>133333</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <f t="shared" si="13"/>
+        <v>10</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C100">
+        <v>133333</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <f t="shared" si="13"/>
+        <v>10</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C101">
+        <v>133333</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <f t="shared" si="13"/>
+        <v>10</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C102">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <f t="shared" si="13"/>
+        <v>10</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C103">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <f t="shared" si="13"/>
+        <v>10</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C104">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <f t="shared" si="13"/>
+        <v>10</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C105">
+        <v>26666</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <f t="shared" si="13"/>
+        <v>10</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C106">
+        <v>26666</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <f t="shared" si="13"/>
+        <v>10</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C107">
+        <v>26666</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <f t="shared" si="13"/>
+        <v>10</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C108">
+        <v>3333</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <f t="shared" si="13"/>
+        <v>10</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C109">
+        <v>3333</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <f t="shared" si="13"/>
+        <v>10</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C110">
+        <v>3333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>